<commit_message>
fix: altera schema para permitir insercao de dados mesmo que estejam inconsistentes com as regras de negocio da Receita Federal
</commit_message>
<xml_diff>
--- a/sql/fonte_de_dados.xlsx
+++ b/sql/fonte_de_dados.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t xml:space="preserve">tabela</t>
   </si>
@@ -43,6 +43,9 @@
     <t xml:space="preserve">http://200.152.38.155/CNPJ/F.K03200$Z.D20108.QUALSCSV.zip</t>
   </si>
   <si>
+    <t xml:space="preserve">qualificacao_id = 36 inexistente. Foi inserida como (‘36’, NULL) no banco de dados para evitar de perder essa linha</t>
+  </si>
+  <si>
     <t xml:space="preserve">Porte</t>
   </si>
   <si>
@@ -53,6 +56,29 @@
   </si>
   <si>
     <t xml:space="preserve">http://200.152.38.155/CNPJ/F.K03200$Z.D20108.PAISCSV.zip</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">pais_id = 367 inexistente. Foi inserida como (‘367’, NULL) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">no banco de dados para evitar de perder essa linha
+idem para pais_id = 150
+idem para pais_id = 449
+idem para pais_id = 678
+idem para pais_id = 359</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">FaixaEtaria</t>
@@ -113,7 +139,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -134,6 +160,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -178,9 +209,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -202,15 +237,15 @@
   </sheetPr>
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="116.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="49.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="91.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -239,10 +274,13 @@
       <c r="B3" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="C3" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>4</v>
@@ -250,31 +288,34 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="58.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>4</v>
@@ -282,7 +323,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>4</v>
@@ -290,53 +331,53 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>